<commit_message>
Add lifecycle of mineral discovery diagram to £KOD
</commit_message>
<xml_diff>
--- a/£KOD.xlsx
+++ b/£KOD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A8CAAF0-AE71-C149-97C9-09BEF03C5C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41222E9E-7307-FB47-9E7F-E5BEF074ADC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18920" xr2:uid="{8724097C-16E9-4DD8-A664-E92B012AA13F}"/>
   </bookViews>
@@ -191,7 +191,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
-    <numFmt numFmtId="168" formatCode="#,##0.000"/>
+    <numFmt numFmtId="166" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -423,27 +423,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -466,15 +445,36 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -538,6 +538,67 @@
         <a:xfrm>
           <a:off x="3009901" y="101601"/>
           <a:ext cx="876299" cy="809745"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>397932</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>503766</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B61F7FC1-2A22-2DE2-68D6-A46A8E3F633B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="397932" y="6934200"/>
+          <a:ext cx="11281834" cy="6769100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -858,8 +919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89539D8F-2E0A-4B42-BC33-C56645A0E544}">
   <dimension ref="A2:Z41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S35" sqref="S35:S37"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="R78" sqref="R78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -872,12 +933,12 @@
         <v>0</v>
       </c>
       <c r="E2"/>
-      <c r="G2" s="35" t="s">
+      <c r="G2" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
     </row>
     <row r="3" spans="2:26" x14ac:dyDescent="0.15">
       <c r="B3" s="2" t="s">
@@ -885,32 +946,32 @@
       </c>
     </row>
     <row r="6" spans="2:26" x14ac:dyDescent="0.15">
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="22"/>
-      <c r="G6" s="20" t="s">
+      <c r="C6" s="38"/>
+      <c r="D6" s="39"/>
+      <c r="G6" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="21"/>
-      <c r="M6" s="21"/>
-      <c r="N6" s="21"/>
-      <c r="O6" s="21"/>
-      <c r="P6" s="21"/>
-      <c r="Q6" s="21"/>
-      <c r="R6" s="21"/>
-      <c r="S6" s="22"/>
-      <c r="V6" s="20" t="s">
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="38"/>
+      <c r="L6" s="38"/>
+      <c r="M6" s="38"/>
+      <c r="N6" s="38"/>
+      <c r="O6" s="38"/>
+      <c r="P6" s="38"/>
+      <c r="Q6" s="38"/>
+      <c r="R6" s="38"/>
+      <c r="S6" s="39"/>
+      <c r="V6" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="W6" s="21"/>
-      <c r="X6" s="21"/>
-      <c r="Y6" s="22"/>
+      <c r="W6" s="38"/>
+      <c r="X6" s="38"/>
+      <c r="Y6" s="39"/>
     </row>
     <row r="7" spans="2:26" x14ac:dyDescent="0.15">
       <c r="B7" s="4" t="s">
@@ -921,27 +982,27 @@
       </c>
       <c r="D7" s="16"/>
       <c r="G7" s="12"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
-      <c r="L7" s="25"/>
-      <c r="M7" s="25"/>
-      <c r="N7" s="25"/>
-      <c r="O7" s="25"/>
-      <c r="P7" s="25"/>
-      <c r="Q7" s="25"/>
-      <c r="R7" s="25"/>
-      <c r="S7" s="26"/>
-      <c r="V7" s="29" t="s">
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="18"/>
+      <c r="Q7" s="18"/>
+      <c r="R7" s="18"/>
+      <c r="S7" s="19"/>
+      <c r="V7" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="W7" s="25"/>
-      <c r="X7" s="25"/>
-      <c r="Y7" s="34" t="s">
+      <c r="W7" s="18"/>
+      <c r="X7" s="18"/>
+      <c r="Y7" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="Z7" s="44" t="s">
+      <c r="Z7" s="35" t="s">
         <v>41</v>
       </c>
     </row>
@@ -956,24 +1017,24 @@
         <v>37</v>
       </c>
       <c r="G8" s="12"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="25"/>
-      <c r="N8" s="25"/>
-      <c r="O8" s="25"/>
-      <c r="P8" s="25"/>
-      <c r="Q8" s="25"/>
-      <c r="R8" s="25"/>
-      <c r="S8" s="26"/>
-      <c r="V8" s="32" t="s">
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="18"/>
+      <c r="Q8" s="18"/>
+      <c r="R8" s="18"/>
+      <c r="S8" s="19"/>
+      <c r="V8" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="W8" s="25"/>
-      <c r="X8" s="25"/>
-      <c r="Y8" s="26"/>
+      <c r="W8" s="18"/>
+      <c r="X8" s="18"/>
+      <c r="Y8" s="19"/>
     </row>
     <row r="9" spans="2:26" x14ac:dyDescent="0.15">
       <c r="B9" s="4" t="s">
@@ -984,30 +1045,30 @@
         <v>40.728999999999999</v>
       </c>
       <c r="D9" s="16"/>
-      <c r="E9" s="37"/>
-      <c r="G9" s="38">
+      <c r="E9" s="30"/>
+      <c r="G9" s="31">
         <v>44805</v>
       </c>
-      <c r="H9" s="39" t="s">
+      <c r="H9" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="25"/>
-      <c r="L9" s="25"/>
-      <c r="M9" s="25"/>
-      <c r="N9" s="25"/>
-      <c r="O9" s="25"/>
-      <c r="P9" s="25"/>
-      <c r="Q9" s="25"/>
-      <c r="R9" s="25"/>
-      <c r="S9" s="26"/>
-      <c r="V9" s="32" t="s">
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="18"/>
+      <c r="Q9" s="18"/>
+      <c r="R9" s="18"/>
+      <c r="S9" s="19"/>
+      <c r="V9" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="W9" s="25"/>
-      <c r="X9" s="25"/>
-      <c r="Y9" s="26"/>
+      <c r="W9" s="18"/>
+      <c r="X9" s="18"/>
+      <c r="Y9" s="19"/>
     </row>
     <row r="10" spans="2:26" x14ac:dyDescent="0.15">
       <c r="B10" s="4" t="s">
@@ -1019,26 +1080,26 @@
       <c r="D10" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="45"/>
+      <c r="E10" s="36"/>
       <c r="G10" s="12"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="25"/>
-      <c r="O10" s="25"/>
-      <c r="P10" s="25"/>
-      <c r="Q10" s="25"/>
-      <c r="R10" s="25"/>
-      <c r="S10" s="26"/>
-      <c r="V10" s="33" t="s">
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18"/>
+      <c r="R10" s="18"/>
+      <c r="S10" s="19"/>
+      <c r="V10" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="W10" s="25"/>
-      <c r="X10" s="25"/>
-      <c r="Y10" s="26"/>
+      <c r="W10" s="18"/>
+      <c r="X10" s="18"/>
+      <c r="Y10" s="19"/>
     </row>
     <row r="11" spans="2:26" x14ac:dyDescent="0.15">
       <c r="B11" s="4" t="s">
@@ -1051,22 +1112,22 @@
         <v>37</v>
       </c>
       <c r="G11" s="12"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25"/>
-      <c r="N11" s="25"/>
-      <c r="O11" s="25"/>
-      <c r="P11" s="25"/>
-      <c r="Q11" s="25"/>
-      <c r="R11" s="25"/>
-      <c r="S11" s="26"/>
-      <c r="V11" s="30"/>
-      <c r="W11" s="25"/>
-      <c r="X11" s="25"/>
-      <c r="Y11" s="26"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="18"/>
+      <c r="P11" s="18"/>
+      <c r="Q11" s="18"/>
+      <c r="R11" s="18"/>
+      <c r="S11" s="19"/>
+      <c r="V11" s="23"/>
+      <c r="W11" s="18"/>
+      <c r="X11" s="18"/>
+      <c r="Y11" s="19"/>
     </row>
     <row r="12" spans="2:26" x14ac:dyDescent="0.15">
       <c r="B12" s="4" t="s">
@@ -1080,22 +1141,22 @@
         <v>37</v>
       </c>
       <c r="G12" s="12"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="25"/>
-      <c r="O12" s="25"/>
-      <c r="P12" s="25"/>
-      <c r="Q12" s="25"/>
-      <c r="R12" s="25"/>
-      <c r="S12" s="26"/>
-      <c r="V12" s="30"/>
-      <c r="W12" s="25"/>
-      <c r="X12" s="25"/>
-      <c r="Y12" s="26"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="18"/>
+      <c r="P12" s="18"/>
+      <c r="Q12" s="18"/>
+      <c r="R12" s="18"/>
+      <c r="S12" s="19"/>
+      <c r="V12" s="23"/>
+      <c r="W12" s="18"/>
+      <c r="X12" s="18"/>
+      <c r="Y12" s="19"/>
     </row>
     <row r="13" spans="2:26" x14ac:dyDescent="0.15">
       <c r="B13" s="5" t="s">
@@ -1107,337 +1168,338 @@
       </c>
       <c r="D13" s="17"/>
       <c r="G13" s="12"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="25"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="25"/>
-      <c r="M13" s="25"/>
-      <c r="N13" s="25"/>
-      <c r="O13" s="25"/>
-      <c r="P13" s="25"/>
-      <c r="Q13" s="25"/>
-      <c r="R13" s="25"/>
-      <c r="S13" s="26"/>
-      <c r="V13" s="30"/>
-      <c r="W13" s="25"/>
-      <c r="X13" s="25"/>
-      <c r="Y13" s="26"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="18"/>
+      <c r="N13" s="18"/>
+      <c r="O13" s="18"/>
+      <c r="P13" s="18"/>
+      <c r="Q13" s="18"/>
+      <c r="R13" s="18"/>
+      <c r="S13" s="19"/>
+      <c r="V13" s="23"/>
+      <c r="W13" s="18"/>
+      <c r="X13" s="18"/>
+      <c r="Y13" s="19"/>
     </row>
     <row r="14" spans="2:26" x14ac:dyDescent="0.15">
       <c r="G14" s="12"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="25"/>
-      <c r="L14" s="25"/>
-      <c r="M14" s="25"/>
-      <c r="N14" s="25"/>
-      <c r="O14" s="25"/>
-      <c r="P14" s="25"/>
-      <c r="Q14" s="25"/>
-      <c r="R14" s="25"/>
-      <c r="S14" s="26"/>
-      <c r="V14" s="30"/>
-      <c r="W14" s="25"/>
-      <c r="X14" s="25"/>
-      <c r="Y14" s="26"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="18"/>
+      <c r="O14" s="18"/>
+      <c r="P14" s="18"/>
+      <c r="Q14" s="18"/>
+      <c r="R14" s="18"/>
+      <c r="S14" s="19"/>
+      <c r="V14" s="23"/>
+      <c r="W14" s="18"/>
+      <c r="X14" s="18"/>
+      <c r="Y14" s="19"/>
     </row>
     <row r="15" spans="2:26" x14ac:dyDescent="0.15">
       <c r="G15" s="12"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="25"/>
-      <c r="L15" s="25"/>
-      <c r="M15" s="25"/>
-      <c r="N15" s="25"/>
-      <c r="O15" s="25"/>
-      <c r="P15" s="25"/>
-      <c r="Q15" s="25"/>
-      <c r="R15" s="25"/>
-      <c r="S15" s="26"/>
-      <c r="V15" s="30"/>
-      <c r="W15" s="25"/>
-      <c r="X15" s="25"/>
-      <c r="Y15" s="26"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="18"/>
+      <c r="O15" s="18"/>
+      <c r="P15" s="18"/>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="18"/>
+      <c r="S15" s="19"/>
+      <c r="V15" s="23"/>
+      <c r="W15" s="18"/>
+      <c r="X15" s="18"/>
+      <c r="Y15" s="19"/>
     </row>
     <row r="16" spans="2:26" x14ac:dyDescent="0.15">
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="22"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="39"/>
       <c r="G16" s="12"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="25"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="25"/>
-      <c r="L16" s="25"/>
-      <c r="M16" s="25"/>
-      <c r="N16" s="25"/>
-      <c r="O16" s="25"/>
-      <c r="P16" s="25"/>
-      <c r="Q16" s="25"/>
-      <c r="R16" s="25"/>
-      <c r="S16" s="26"/>
-      <c r="V16" s="30"/>
-      <c r="W16" s="25"/>
-      <c r="X16" s="25"/>
-      <c r="Y16" s="26"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
+      <c r="N16" s="18"/>
+      <c r="O16" s="18"/>
+      <c r="P16" s="18"/>
+      <c r="Q16" s="18"/>
+      <c r="R16" s="18"/>
+      <c r="S16" s="19"/>
+      <c r="V16" s="23"/>
+      <c r="W16" s="18"/>
+      <c r="X16" s="18"/>
+      <c r="Y16" s="19"/>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A17" s="11"/>
       <c r="B17" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="23" t="s">
+      <c r="C17" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="24"/>
+      <c r="D17" s="43"/>
       <c r="E17" s="1" t="s">
         <v>18</v>
       </c>
       <c r="G17" s="12"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="25"/>
-      <c r="L17" s="25"/>
-      <c r="M17" s="25"/>
-      <c r="N17" s="25"/>
-      <c r="O17" s="25"/>
-      <c r="P17" s="25"/>
-      <c r="Q17" s="25"/>
-      <c r="R17" s="25"/>
-      <c r="S17" s="26"/>
-      <c r="V17" s="31"/>
-      <c r="W17" s="27"/>
-      <c r="X17" s="27"/>
-      <c r="Y17" s="28"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="18"/>
+      <c r="N17" s="18"/>
+      <c r="O17" s="18"/>
+      <c r="P17" s="18"/>
+      <c r="Q17" s="18"/>
+      <c r="R17" s="18"/>
+      <c r="S17" s="19"/>
+      <c r="V17" s="24"/>
+      <c r="W17" s="20"/>
+      <c r="X17" s="20"/>
+      <c r="Y17" s="21"/>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A18" s="11"/>
       <c r="B18" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="23"/>
-      <c r="D18" s="24"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="43"/>
       <c r="G18" s="12"/>
-      <c r="H18" s="25"/>
-      <c r="I18" s="25"/>
-      <c r="J18" s="25"/>
-      <c r="K18" s="25"/>
-      <c r="L18" s="25"/>
-      <c r="M18" s="25"/>
-      <c r="N18" s="25"/>
-      <c r="O18" s="25"/>
-      <c r="P18" s="25"/>
-      <c r="Q18" s="25"/>
-      <c r="R18" s="25"/>
-      <c r="S18" s="26"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
+      <c r="M18" s="18"/>
+      <c r="N18" s="18"/>
+      <c r="O18" s="18"/>
+      <c r="P18" s="18"/>
+      <c r="Q18" s="18"/>
+      <c r="R18" s="18"/>
+      <c r="S18" s="19"/>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A19" s="11"/>
       <c r="B19" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="23" t="s">
+      <c r="C19" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="24"/>
+      <c r="D19" s="43"/>
       <c r="E19" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G19" s="12"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="25"/>
-      <c r="K19" s="25"/>
-      <c r="L19" s="25"/>
-      <c r="M19" s="25"/>
-      <c r="N19" s="25"/>
-      <c r="O19" s="25"/>
-      <c r="P19" s="25"/>
-      <c r="Q19" s="25"/>
-      <c r="R19" s="25"/>
-      <c r="S19" s="26"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="18"/>
+      <c r="M19" s="18"/>
+      <c r="N19" s="18"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="18"/>
+      <c r="Q19" s="18"/>
+      <c r="R19" s="18"/>
+      <c r="S19" s="19"/>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A20" s="11"/>
       <c r="B20" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="19"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="41"/>
       <c r="G20" s="12"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="25"/>
-      <c r="J20" s="25"/>
-      <c r="K20" s="25"/>
-      <c r="L20" s="25"/>
-      <c r="M20" s="25"/>
-      <c r="N20" s="25"/>
-      <c r="O20" s="25"/>
-      <c r="P20" s="25"/>
-      <c r="Q20" s="25"/>
-      <c r="R20" s="25"/>
-      <c r="S20" s="26"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="18"/>
+      <c r="O20" s="18"/>
+      <c r="P20" s="18"/>
+      <c r="Q20" s="18"/>
+      <c r="R20" s="18"/>
+      <c r="S20" s="19"/>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.15">
       <c r="G21" s="12"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="25"/>
-      <c r="K21" s="25"/>
-      <c r="L21" s="25"/>
-      <c r="M21" s="25"/>
-      <c r="N21" s="25"/>
-      <c r="O21" s="25"/>
-      <c r="P21" s="25"/>
-      <c r="Q21" s="25"/>
-      <c r="R21" s="25"/>
-      <c r="S21" s="26"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="18"/>
+      <c r="O21" s="18"/>
+      <c r="P21" s="18"/>
+      <c r="Q21" s="18"/>
+      <c r="R21" s="18"/>
+      <c r="S21" s="19"/>
       <c r="V21" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.15">
       <c r="G22" s="12"/>
-      <c r="H22" s="25"/>
-      <c r="I22" s="25"/>
-      <c r="J22" s="25"/>
-      <c r="K22" s="25"/>
-      <c r="L22" s="25"/>
-      <c r="M22" s="25"/>
-      <c r="N22" s="25"/>
-      <c r="O22" s="25"/>
-      <c r="P22" s="25"/>
-      <c r="Q22" s="25"/>
-      <c r="R22" s="25"/>
-      <c r="S22" s="26"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="18"/>
+      <c r="N22" s="18"/>
+      <c r="O22" s="18"/>
+      <c r="P22" s="18"/>
+      <c r="Q22" s="18"/>
+      <c r="R22" s="18"/>
+      <c r="S22" s="19"/>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="21"/>
-      <c r="D23" s="22"/>
-      <c r="G23" s="38">
+      <c r="C23" s="38"/>
+      <c r="D23" s="39"/>
+      <c r="G23" s="31">
         <v>44317</v>
       </c>
-      <c r="H23" s="39" t="s">
+      <c r="H23" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="I23" s="25"/>
-      <c r="J23" s="25"/>
-      <c r="K23" s="25"/>
-      <c r="L23" s="25"/>
-      <c r="M23" s="25"/>
-      <c r="N23" s="25"/>
-      <c r="O23" s="25"/>
-      <c r="P23" s="25"/>
-      <c r="Q23" s="25"/>
-      <c r="R23" s="25"/>
-      <c r="S23" s="26"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="18"/>
+      <c r="O23" s="18"/>
+      <c r="P23" s="18"/>
+      <c r="Q23" s="18"/>
+      <c r="R23" s="18"/>
+      <c r="S23" s="19"/>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.15">
       <c r="B24" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="23" t="s">
+      <c r="C24" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="24"/>
+      <c r="D24" s="43"/>
       <c r="G24" s="12"/>
-      <c r="H24" s="25"/>
-      <c r="I24" s="25"/>
-      <c r="J24" s="25"/>
-      <c r="K24" s="25"/>
-      <c r="L24" s="25"/>
-      <c r="M24" s="25"/>
-      <c r="N24" s="25"/>
-      <c r="O24" s="25"/>
-      <c r="P24" s="25"/>
-      <c r="Q24" s="25"/>
-      <c r="R24" s="25"/>
-      <c r="S24" s="26"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="18"/>
+      <c r="P24" s="18"/>
+      <c r="Q24" s="18"/>
+      <c r="R24" s="18"/>
+      <c r="S24" s="19"/>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.15">
       <c r="B25" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="23">
+      <c r="C25" s="42">
         <v>2010</v>
       </c>
-      <c r="D25" s="24"/>
+      <c r="D25" s="43"/>
       <c r="G25" s="12"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="25"/>
-      <c r="J25" s="25"/>
-      <c r="K25" s="25"/>
-      <c r="L25" s="25"/>
-      <c r="M25" s="25"/>
-      <c r="N25" s="25"/>
-      <c r="O25" s="25"/>
-      <c r="P25" s="25"/>
-      <c r="Q25" s="25"/>
-      <c r="R25" s="25"/>
-      <c r="S25" s="26"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
+      <c r="M25" s="18"/>
+      <c r="N25" s="18"/>
+      <c r="O25" s="18"/>
+      <c r="P25" s="18"/>
+      <c r="Q25" s="18"/>
+      <c r="R25" s="18"/>
+      <c r="S25" s="19"/>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.15">
       <c r="B26" s="12"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="24"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="43"/>
       <c r="G26" s="12"/>
-      <c r="H26" s="25"/>
-      <c r="I26" s="25"/>
-      <c r="J26" s="25"/>
-      <c r="K26" s="25"/>
-      <c r="L26" s="25"/>
-      <c r="M26" s="25"/>
-      <c r="N26" s="25"/>
-      <c r="O26" s="25"/>
-      <c r="P26" s="25"/>
-      <c r="Q26" s="25"/>
-      <c r="R26" s="25"/>
-      <c r="S26" s="26"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="18"/>
+      <c r="N26" s="18"/>
+      <c r="O26" s="18"/>
+      <c r="P26" s="18"/>
+      <c r="Q26" s="18"/>
+      <c r="R26" s="18"/>
+      <c r="S26" s="19"/>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.15">
       <c r="B27" s="12"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="24"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="43"/>
       <c r="G27" s="12"/>
-      <c r="H27" s="25"/>
-      <c r="I27" s="25"/>
-      <c r="J27" s="25"/>
-      <c r="K27" s="25"/>
-      <c r="L27" s="25"/>
-      <c r="M27" s="25"/>
-      <c r="N27" s="25"/>
-      <c r="O27" s="25"/>
-      <c r="P27" s="25"/>
-      <c r="Q27" s="25"/>
-      <c r="R27" s="25"/>
-      <c r="S27" s="26"/>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="18"/>
+      <c r="M27" s="18"/>
+      <c r="N27" s="18"/>
+      <c r="O27" s="18"/>
+      <c r="P27" s="18"/>
+      <c r="Q27" s="18"/>
+      <c r="R27" s="18"/>
+      <c r="S27" s="19"/>
+    </row>
+    <row r="28" spans="1:25" ht="15" x14ac:dyDescent="0.2">
       <c r="B28" s="12"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="24"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="43"/>
       <c r="G28" s="12"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
-      <c r="K28" s="25"/>
-      <c r="L28" s="25"/>
-      <c r="M28" s="25"/>
-      <c r="N28" s="25"/>
-      <c r="O28" s="25"/>
-      <c r="P28" s="25"/>
-      <c r="Q28" s="25"/>
-      <c r="R28" s="25"/>
-      <c r="S28" s="26"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="18"/>
+      <c r="M28" s="18"/>
+      <c r="N28" s="18"/>
+      <c r="O28" s="18"/>
+      <c r="P28" s="18"/>
+      <c r="Q28" s="18"/>
+      <c r="R28" s="18"/>
+      <c r="S28" s="19"/>
+      <c r="V28"/>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.15">
       <c r="B29" s="12" t="s">
@@ -1446,43 +1508,43 @@
       <c r="C29" s="14"/>
       <c r="D29" s="15"/>
       <c r="G29" s="12"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
-      <c r="K29" s="25"/>
-      <c r="L29" s="25"/>
-      <c r="M29" s="25"/>
-      <c r="N29" s="25"/>
-      <c r="O29" s="25"/>
-      <c r="P29" s="25"/>
-      <c r="Q29" s="25"/>
-      <c r="R29" s="25"/>
-      <c r="S29" s="26"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="18"/>
+      <c r="M29" s="18"/>
+      <c r="N29" s="18"/>
+      <c r="O29" s="18"/>
+      <c r="P29" s="18"/>
+      <c r="Q29" s="18"/>
+      <c r="R29" s="18"/>
+      <c r="S29" s="19"/>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.15">
       <c r="B30" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="41" t="s">
+      <c r="C30" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="D30" s="42"/>
+      <c r="D30" s="45"/>
       <c r="G30" s="13"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
-      <c r="K30" s="27"/>
-      <c r="L30" s="27"/>
-      <c r="M30" s="27"/>
-      <c r="N30" s="27"/>
-      <c r="O30" s="27"/>
-      <c r="P30" s="27"/>
-      <c r="Q30" s="27"/>
-      <c r="R30" s="27"/>
-      <c r="S30" s="28"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
+      <c r="K30" s="20"/>
+      <c r="L30" s="20"/>
+      <c r="M30" s="20"/>
+      <c r="N30" s="20"/>
+      <c r="O30" s="20"/>
+      <c r="P30" s="20"/>
+      <c r="Q30" s="20"/>
+      <c r="R30" s="20"/>
+      <c r="S30" s="21"/>
     </row>
     <row r="34" spans="3:19" x14ac:dyDescent="0.15">
-      <c r="G34" s="36" t="s">
+      <c r="G34" s="29" t="s">
         <v>33</v>
       </c>
       <c r="R34" s="2" t="s">
@@ -1490,22 +1552,22 @@
       </c>
     </row>
     <row r="35" spans="3:19" x14ac:dyDescent="0.15">
-      <c r="C35" s="40"/>
+      <c r="C35" s="33"/>
       <c r="R35" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="S35" s="43" t="s">
+      <c r="S35" s="34" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="36" spans="3:19" x14ac:dyDescent="0.15">
-      <c r="G36" s="36" t="s">
+      <c r="G36" s="29" t="s">
         <v>39</v>
       </c>
       <c r="R36" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="S36" s="43" t="s">
+      <c r="S36" s="34" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1513,12 +1575,12 @@
       <c r="R37" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="S37" s="43" t="s">
+      <c r="S37" s="34" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="38" spans="3:19" x14ac:dyDescent="0.15">
-      <c r="P38" s="37"/>
+      <c r="P38" s="30"/>
     </row>
     <row r="41" spans="3:19" x14ac:dyDescent="0.15">
       <c r="G41" s="1" t="s">
@@ -1527,6 +1589,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
     <mergeCell ref="G6:S6"/>
     <mergeCell ref="V6:Y6"/>
     <mergeCell ref="B6:D6"/>
@@ -1535,13 +1604,6 @@
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H9" r:id="rId1" xr:uid="{77F3DFC6-F58B-5C44-BDC9-407B8FA9A543}"/>

</xml_diff>

<commit_message>
£KOD news of financing & JV
</commit_message>
<xml_diff>
--- a/£KOD.xlsx
+++ b/£KOD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41222E9E-7307-FB47-9E7F-E5BEF074ADC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC8B24A-5D19-48FB-AB8F-D92726E951F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18920" xr2:uid="{8724097C-16E9-4DD8-A664-E92B012AA13F}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="33600" windowHeight="18915" xr2:uid="{8724097C-16E9-4DD8-A664-E92B012AA13F}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -20,22 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="50">
   <si>
     <t>£KOD</t>
   </si>
@@ -182,6 +172,9 @@
   </si>
   <si>
     <t>Funding Options:</t>
+  </si>
+  <si>
+    <t>Kodal Minerals spikes +60% on news of $117.75m funding secured via a Joint Venture to fully finance lithium project</t>
   </si>
 </sst>
 </file>
@@ -448,6 +441,12 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -457,22 +456,16 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -919,16 +912,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89539D8F-2E0A-4B42-BC33-C56645A0E544}">
   <dimension ref="A2:Z41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="R78" sqref="R78"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:26" ht="15" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -940,40 +933,40 @@
       <c r="I2" s="28"/>
       <c r="J2" s="28"/>
     </row>
-    <row r="3" spans="2:26" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:26" x14ac:dyDescent="0.15">
-      <c r="B6" s="37" t="s">
+    <row r="6" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B6" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="39"/>
-      <c r="G6" s="37" t="s">
+      <c r="C6" s="40"/>
+      <c r="D6" s="41"/>
+      <c r="G6" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="38"/>
-      <c r="K6" s="38"/>
-      <c r="L6" s="38"/>
-      <c r="M6" s="38"/>
-      <c r="N6" s="38"/>
-      <c r="O6" s="38"/>
-      <c r="P6" s="38"/>
-      <c r="Q6" s="38"/>
-      <c r="R6" s="38"/>
-      <c r="S6" s="39"/>
-      <c r="V6" s="37" t="s">
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="40"/>
+      <c r="N6" s="40"/>
+      <c r="O6" s="40"/>
+      <c r="P6" s="40"/>
+      <c r="Q6" s="40"/>
+      <c r="R6" s="40"/>
+      <c r="S6" s="41"/>
+      <c r="V6" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="W6" s="38"/>
-      <c r="X6" s="38"/>
-      <c r="Y6" s="39"/>
-    </row>
-    <row r="7" spans="2:26" x14ac:dyDescent="0.15">
+      <c r="W6" s="40"/>
+      <c r="X6" s="40"/>
+      <c r="Y6" s="41"/>
+    </row>
+    <row r="7" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
@@ -1006,7 +999,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="2:26" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
@@ -1036,7 +1029,7 @@
       <c r="X8" s="18"/>
       <c r="Y8" s="19"/>
     </row>
-    <row r="9" spans="2:26" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="s">
         <v>5</v>
       </c>
@@ -1047,12 +1040,11 @@
       <c r="D9" s="16"/>
       <c r="E9" s="30"/>
       <c r="G9" s="31">
-        <v>44805</v>
+        <v>44927</v>
       </c>
       <c r="H9" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="I9" s="18"/>
+        <v>49</v>
+      </c>
       <c r="J9" s="18"/>
       <c r="K9" s="18"/>
       <c r="L9" s="18"/>
@@ -1070,7 +1062,7 @@
       <c r="X9" s="18"/>
       <c r="Y9" s="19"/>
     </row>
-    <row r="10" spans="2:26" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B10" s="4" t="s">
         <v>6</v>
       </c>
@@ -1101,7 +1093,7 @@
       <c r="X10" s="18"/>
       <c r="Y10" s="19"/>
     </row>
-    <row r="11" spans="2:26" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B11" s="4" t="s">
         <v>7</v>
       </c>
@@ -1129,7 +1121,7 @@
       <c r="X11" s="18"/>
       <c r="Y11" s="19"/>
     </row>
-    <row r="12" spans="2:26" x14ac:dyDescent="0.15">
+    <row r="12" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B12" s="4" t="s">
         <v>8</v>
       </c>
@@ -1158,7 +1150,7 @@
       <c r="X12" s="18"/>
       <c r="Y12" s="19"/>
     </row>
-    <row r="13" spans="2:26" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B13" s="5" t="s">
         <v>9</v>
       </c>
@@ -1185,7 +1177,7 @@
       <c r="X13" s="18"/>
       <c r="Y13" s="19"/>
     </row>
-    <row r="14" spans="2:26" x14ac:dyDescent="0.15">
+    <row r="14" spans="2:26" x14ac:dyDescent="0.2">
       <c r="G14" s="12"/>
       <c r="H14" s="18"/>
       <c r="I14" s="18"/>
@@ -1204,9 +1196,13 @@
       <c r="X14" s="18"/>
       <c r="Y14" s="19"/>
     </row>
-    <row r="15" spans="2:26" x14ac:dyDescent="0.15">
-      <c r="G15" s="12"/>
-      <c r="H15" s="18"/>
+    <row r="15" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="G15" s="31">
+        <v>44805</v>
+      </c>
+      <c r="H15" s="32" t="s">
+        <v>34</v>
+      </c>
       <c r="I15" s="18"/>
       <c r="J15" s="18"/>
       <c r="K15" s="18"/>
@@ -1223,12 +1219,12 @@
       <c r="X15" s="18"/>
       <c r="Y15" s="19"/>
     </row>
-    <row r="16" spans="2:26" x14ac:dyDescent="0.15">
-      <c r="B16" s="37" t="s">
+    <row r="16" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B16" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="39"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="41"/>
       <c r="G16" s="12"/>
       <c r="H16" s="18"/>
       <c r="I16" s="18"/>
@@ -1247,7 +1243,7 @@
       <c r="X16" s="18"/>
       <c r="Y16" s="19"/>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" s="11"/>
       <c r="B17" s="9" t="s">
         <v>11</v>
@@ -1277,7 +1273,7 @@
       <c r="X17" s="20"/>
       <c r="Y17" s="21"/>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" s="11"/>
       <c r="B18" s="9" t="s">
         <v>12</v>
@@ -1298,7 +1294,7 @@
       <c r="R18" s="18"/>
       <c r="S18" s="19"/>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" s="11"/>
       <c r="B19" s="9" t="s">
         <v>13</v>
@@ -1324,13 +1320,13 @@
       <c r="R19" s="18"/>
       <c r="S19" s="19"/>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20" s="11"/>
       <c r="B20" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="40"/>
-      <c r="D20" s="41"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="45"/>
       <c r="G20" s="12"/>
       <c r="H20" s="18"/>
       <c r="I20" s="18"/>
@@ -1345,7 +1341,7 @@
       <c r="R20" s="18"/>
       <c r="S20" s="19"/>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="G21" s="12"/>
       <c r="H21" s="18"/>
       <c r="I21" s="18"/>
@@ -1363,7 +1359,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="G22" s="12"/>
       <c r="H22" s="18"/>
       <c r="I22" s="18"/>
@@ -1378,12 +1374,12 @@
       <c r="R22" s="18"/>
       <c r="S22" s="19"/>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="B23" s="37" t="s">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B23" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="38"/>
-      <c r="D23" s="39"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="41"/>
       <c r="G23" s="31">
         <v>44317</v>
       </c>
@@ -1402,7 +1398,7 @@
       <c r="R23" s="18"/>
       <c r="S23" s="19"/>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B24" s="12" t="s">
         <v>20</v>
       </c>
@@ -1424,7 +1420,7 @@
       <c r="R24" s="18"/>
       <c r="S24" s="19"/>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B25" s="12" t="s">
         <v>21</v>
       </c>
@@ -1446,7 +1442,7 @@
       <c r="R25" s="18"/>
       <c r="S25" s="19"/>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B26" s="12"/>
       <c r="C26" s="42"/>
       <c r="D26" s="43"/>
@@ -1464,7 +1460,7 @@
       <c r="R26" s="18"/>
       <c r="S26" s="19"/>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B27" s="12"/>
       <c r="C27" s="42"/>
       <c r="D27" s="43"/>
@@ -1482,7 +1478,7 @@
       <c r="R27" s="18"/>
       <c r="S27" s="19"/>
     </row>
-    <row r="28" spans="1:25" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="B28" s="12"/>
       <c r="C28" s="42"/>
       <c r="D28" s="43"/>
@@ -1501,7 +1497,7 @@
       <c r="S28" s="19"/>
       <c r="V28"/>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B29" s="12" t="s">
         <v>23</v>
       </c>
@@ -1521,14 +1517,14 @@
       <c r="R29" s="18"/>
       <c r="S29" s="19"/>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B30" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="44" t="s">
+      <c r="C30" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="D30" s="45"/>
+      <c r="D30" s="38"/>
       <c r="G30" s="13"/>
       <c r="H30" s="20"/>
       <c r="I30" s="20"/>
@@ -1543,7 +1539,7 @@
       <c r="R30" s="20"/>
       <c r="S30" s="21"/>
     </row>
-    <row r="34" spans="3:19" x14ac:dyDescent="0.15">
+    <row r="34" spans="3:19" x14ac:dyDescent="0.2">
       <c r="G34" s="29" t="s">
         <v>33</v>
       </c>
@@ -1551,7 +1547,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="3:19" x14ac:dyDescent="0.15">
+    <row r="35" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C35" s="33"/>
       <c r="R35" s="1" t="s">
         <v>46</v>
@@ -1560,7 +1556,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="3:19" x14ac:dyDescent="0.15">
+    <row r="36" spans="3:19" x14ac:dyDescent="0.2">
       <c r="G36" s="29" t="s">
         <v>39</v>
       </c>
@@ -1571,7 +1567,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="3:19" x14ac:dyDescent="0.15">
+    <row r="37" spans="3:19" x14ac:dyDescent="0.2">
       <c r="R37" s="1" t="s">
         <v>43</v>
       </c>
@@ -1579,23 +1575,16 @@
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="3:19" x14ac:dyDescent="0.15">
+    <row r="38" spans="3:19" x14ac:dyDescent="0.2">
       <c r="P38" s="30"/>
     </row>
-    <row r="41" spans="3:19" x14ac:dyDescent="0.15">
+    <row r="41" spans="3:19" x14ac:dyDescent="0.2">
       <c r="G41" s="1" t="s">
         <v>36</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
     <mergeCell ref="G6:S6"/>
     <mergeCell ref="V6:Y6"/>
     <mergeCell ref="B6:D6"/>
@@ -1604,14 +1593,22 @@
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H9" r:id="rId1" xr:uid="{77F3DFC6-F58B-5C44-BDC9-407B8FA9A543}"/>
+    <hyperlink ref="H15" r:id="rId1" xr:uid="{77F3DFC6-F58B-5C44-BDC9-407B8FA9A543}"/>
     <hyperlink ref="C30:D30" r:id="rId2" display="Link" xr:uid="{336D676D-4F82-B242-AB61-E9CB8CE40EDD}"/>
     <hyperlink ref="H23" r:id="rId3" display="2021 Malian coup d'etat begins led by the Malian Army &amp; Vice President of Mali" xr:uid="{98DA3C71-ACDA-5847-9BCE-1CF7AA6AF31A}"/>
+    <hyperlink ref="H9" r:id="rId4" xr:uid="{CFBE2DC5-BD46-4AEA-B124-0F71050A4DEA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
-  <drawing r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <drawing r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Create Lithium explorers overview
</commit_message>
<xml_diff>
--- a/£KOD.xlsx
+++ b/£KOD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{274D9B5A-9A72-424B-8997-20B8A48B4B1C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72F9771-AC14-40C5-8765-429B65C94CA8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="495" windowWidth="33600" windowHeight="18915" xr2:uid="{8724097C-16E9-4DD8-A664-E92B012AA13F}"/>
   </bookViews>
@@ -444,31 +444,31 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -943,32 +943,32 @@
       </c>
     </row>
     <row r="6" spans="2:26" x14ac:dyDescent="0.2">
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="40"/>
-      <c r="D6" s="41"/>
-      <c r="G6" s="39" t="s">
+      <c r="C6" s="38"/>
+      <c r="D6" s="39"/>
+      <c r="G6" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="40"/>
-      <c r="I6" s="40"/>
-      <c r="J6" s="40"/>
-      <c r="K6" s="40"/>
-      <c r="L6" s="40"/>
-      <c r="M6" s="40"/>
-      <c r="N6" s="40"/>
-      <c r="O6" s="40"/>
-      <c r="P6" s="40"/>
-      <c r="Q6" s="40"/>
-      <c r="R6" s="40"/>
-      <c r="S6" s="41"/>
-      <c r="V6" s="39" t="s">
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="38"/>
+      <c r="L6" s="38"/>
+      <c r="M6" s="38"/>
+      <c r="N6" s="38"/>
+      <c r="O6" s="38"/>
+      <c r="P6" s="38"/>
+      <c r="Q6" s="38"/>
+      <c r="R6" s="38"/>
+      <c r="S6" s="39"/>
+      <c r="V6" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="W6" s="40"/>
-      <c r="X6" s="40"/>
-      <c r="Y6" s="41"/>
+      <c r="W6" s="38"/>
+      <c r="X6" s="38"/>
+      <c r="Y6" s="39"/>
     </row>
     <row r="7" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
@@ -1075,8 +1075,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="7">
-        <f>5.7+1.046</f>
-        <v>6.7460000000000004</v>
+        <v>2</v>
       </c>
       <c r="D10" s="16" t="s">
         <v>37</v>
@@ -1136,7 +1135,7 @@
       </c>
       <c r="C12" s="7">
         <f>C10-C11</f>
-        <v>6.7460000000000004</v>
+        <v>2</v>
       </c>
       <c r="D12" s="16" t="s">
         <v>37</v>
@@ -1165,7 +1164,7 @@
       </c>
       <c r="C13" s="8">
         <f>C9-C12</f>
-        <v>62.544000000000004</v>
+        <v>67.290000000000006</v>
       </c>
       <c r="D13" s="17"/>
       <c r="G13" s="12"/>
@@ -1229,11 +1228,11 @@
       <c r="Y15" s="19"/>
     </row>
     <row r="16" spans="2:26" x14ac:dyDescent="0.2">
-      <c r="B16" s="39" t="s">
+      <c r="B16" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="40"/>
-      <c r="D16" s="41"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="39"/>
       <c r="G16" s="12"/>
       <c r="H16" s="18"/>
       <c r="I16" s="18"/>
@@ -1334,8 +1333,8 @@
       <c r="B20" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="44"/>
-      <c r="D20" s="45"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="41"/>
       <c r="G20" s="12"/>
       <c r="H20" s="18"/>
       <c r="I20" s="18"/>
@@ -1384,11 +1383,11 @@
       <c r="S22" s="19"/>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B23" s="39" t="s">
+      <c r="B23" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="40"/>
-      <c r="D23" s="41"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="39"/>
       <c r="G23" s="31">
         <v>44317</v>
       </c>
@@ -1530,10 +1529,10 @@
       <c r="B30" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="37" t="s">
+      <c r="C30" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="D30" s="38"/>
+      <c r="D30" s="45"/>
       <c r="G30" s="13"/>
       <c r="H30" s="20"/>
       <c r="I30" s="20"/>
@@ -1594,6 +1593,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
     <mergeCell ref="G6:S6"/>
     <mergeCell ref="V6:Y6"/>
     <mergeCell ref="B6:D6"/>
@@ -1602,13 +1608,6 @@
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H15" r:id="rId1" xr:uid="{77F3DFC6-F58B-5C44-BDC9-407B8FA9A543}"/>

</xml_diff>

<commit_message>
£KOD share admission for JV investment
</commit_message>
<xml_diff>
--- a/£KOD.xlsx
+++ b/£KOD.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20396"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{91CF99CF-833B-4C9E-84FC-8632BF756C92}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F53B13EE-C489-4494-889F-309FD5E3BE85}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="495" windowWidth="33600" windowHeight="18915" xr2:uid="{8724097C-16E9-4DD8-A664-E92B012AA13F}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Main" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
   <si>
     <t>£KOD</t>
   </si>
@@ -179,6 +178,9 @@
   </si>
   <si>
     <t>Kodal Minerals confirm receipt of $7 million for JV subsidiary as mentioned in previous finance agreement</t>
+  </si>
+  <si>
+    <t>RNS detailing new admission of shares for JV investment, 106,250,000 new shares added to the total share capital</t>
   </si>
 </sst>
 </file>
@@ -445,31 +447,31 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -917,7 +919,7 @@
   <dimension ref="A2:Z41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -944,46 +946,46 @@
       </c>
     </row>
     <row r="6" spans="2:26" x14ac:dyDescent="0.2">
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="40"/>
-      <c r="D6" s="41"/>
-      <c r="G6" s="39" t="s">
+      <c r="C6" s="38"/>
+      <c r="D6" s="39"/>
+      <c r="G6" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="40"/>
-      <c r="I6" s="40"/>
-      <c r="J6" s="40"/>
-      <c r="K6" s="40"/>
-      <c r="L6" s="40"/>
-      <c r="M6" s="40"/>
-      <c r="N6" s="40"/>
-      <c r="O6" s="40"/>
-      <c r="P6" s="40"/>
-      <c r="Q6" s="40"/>
-      <c r="R6" s="40"/>
-      <c r="S6" s="41"/>
-      <c r="V6" s="39" t="s">
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="38"/>
+      <c r="L6" s="38"/>
+      <c r="M6" s="38"/>
+      <c r="N6" s="38"/>
+      <c r="O6" s="38"/>
+      <c r="P6" s="38"/>
+      <c r="Q6" s="38"/>
+      <c r="R6" s="38"/>
+      <c r="S6" s="39"/>
+      <c r="V6" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="W6" s="40"/>
-      <c r="X6" s="40"/>
-      <c r="Y6" s="41"/>
+      <c r="W6" s="38"/>
+      <c r="X6" s="38"/>
+      <c r="Y6" s="39"/>
     </row>
     <row r="7" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="6">
-        <v>4.1000000000000003E-3</v>
+        <v>3.8999999999999998E-3</v>
       </c>
       <c r="D7" s="16"/>
       <c r="G7" s="31">
-        <v>44958</v>
+        <v>44986</v>
       </c>
       <c r="H7" s="32" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I7" s="18"/>
       <c r="J7" s="18"/>
@@ -1013,7 +1015,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="7">
-        <v>16900</v>
+        <v>17009.980984999998</v>
       </c>
       <c r="D8" s="16" t="s">
         <v>37</v>
@@ -1044,15 +1046,15 @@
       </c>
       <c r="C9" s="7">
         <f>C7*C8</f>
-        <v>69.290000000000006</v>
+        <v>66.338925841499986</v>
       </c>
       <c r="D9" s="16"/>
       <c r="E9" s="30"/>
       <c r="G9" s="31">
-        <v>44927</v>
+        <v>44958</v>
       </c>
       <c r="H9" s="32" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="J9" s="18"/>
       <c r="K9" s="18"/>
@@ -1112,8 +1114,12 @@
       <c r="D11" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="G11" s="12"/>
-      <c r="H11" s="18"/>
+      <c r="G11" s="31">
+        <v>44927</v>
+      </c>
+      <c r="H11" s="32" t="s">
+        <v>48</v>
+      </c>
       <c r="I11" s="18"/>
       <c r="J11" s="18"/>
       <c r="K11" s="18"/>
@@ -1165,7 +1171,7 @@
       </c>
       <c r="C13" s="8">
         <f>C9-C12</f>
-        <v>67.290000000000006</v>
+        <v>64.338925841499986</v>
       </c>
       <c r="D13" s="17"/>
       <c r="G13" s="12"/>
@@ -1206,12 +1212,8 @@
       <c r="Y14" s="19"/>
     </row>
     <row r="15" spans="2:26" x14ac:dyDescent="0.2">
-      <c r="G15" s="31">
-        <v>44805</v>
-      </c>
-      <c r="H15" s="32" t="s">
-        <v>34</v>
-      </c>
+      <c r="G15" s="12"/>
+      <c r="H15" s="18"/>
       <c r="I15" s="18"/>
       <c r="J15" s="18"/>
       <c r="K15" s="18"/>
@@ -1229,11 +1231,11 @@
       <c r="Y15" s="19"/>
     </row>
     <row r="16" spans="2:26" x14ac:dyDescent="0.2">
-      <c r="B16" s="39" t="s">
+      <c r="B16" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="40"/>
-      <c r="D16" s="41"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="39"/>
       <c r="G16" s="12"/>
       <c r="H16" s="18"/>
       <c r="I16" s="18"/>
@@ -1264,8 +1266,12 @@
       <c r="E17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G17" s="12"/>
-      <c r="H17" s="18"/>
+      <c r="G17" s="31">
+        <v>44805</v>
+      </c>
+      <c r="H17" s="32" t="s">
+        <v>34</v>
+      </c>
       <c r="I17" s="18"/>
       <c r="J17" s="18"/>
       <c r="K17" s="18"/>
@@ -1334,8 +1340,8 @@
       <c r="B20" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="44"/>
-      <c r="D20" s="45"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="41"/>
       <c r="G20" s="12"/>
       <c r="H20" s="18"/>
       <c r="I20" s="18"/>
@@ -1384,17 +1390,13 @@
       <c r="S22" s="19"/>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B23" s="39" t="s">
+      <c r="B23" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="40"/>
-      <c r="D23" s="41"/>
-      <c r="G23" s="31">
-        <v>44317</v>
-      </c>
-      <c r="H23" s="32" t="s">
-        <v>38</v>
-      </c>
+      <c r="C23" s="38"/>
+      <c r="D23" s="39"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="18"/>
       <c r="I23" s="18"/>
       <c r="J23" s="18"/>
       <c r="K23" s="18"/>
@@ -1437,8 +1439,12 @@
         <v>2010</v>
       </c>
       <c r="D25" s="43"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="18"/>
+      <c r="G25" s="31">
+        <v>44317</v>
+      </c>
+      <c r="H25" s="32" t="s">
+        <v>38</v>
+      </c>
       <c r="I25" s="18"/>
       <c r="J25" s="18"/>
       <c r="K25" s="18"/>
@@ -1530,10 +1536,10 @@
       <c r="B30" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="37" t="s">
+      <c r="C30" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="D30" s="38"/>
+      <c r="D30" s="45"/>
       <c r="G30" s="13"/>
       <c r="H30" s="20"/>
       <c r="I30" s="20"/>
@@ -1594,6 +1600,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
     <mergeCell ref="G6:S6"/>
     <mergeCell ref="V6:Y6"/>
     <mergeCell ref="B6:D6"/>
@@ -1602,23 +1615,17 @@
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H15" r:id="rId1" xr:uid="{77F3DFC6-F58B-5C44-BDC9-407B8FA9A543}"/>
+    <hyperlink ref="H17" r:id="rId1" xr:uid="{77F3DFC6-F58B-5C44-BDC9-407B8FA9A543}"/>
     <hyperlink ref="C30:D30" r:id="rId2" display="Link" xr:uid="{336D676D-4F82-B242-AB61-E9CB8CE40EDD}"/>
-    <hyperlink ref="H23" r:id="rId3" display="2021 Malian coup d'etat begins led by the Malian Army &amp; Vice President of Mali" xr:uid="{98DA3C71-ACDA-5847-9BCE-1CF7AA6AF31A}"/>
-    <hyperlink ref="H9" r:id="rId4" xr:uid="{CFBE2DC5-BD46-4AEA-B124-0F71050A4DEA}"/>
-    <hyperlink ref="H7" r:id="rId5" display="Kodal Minerals confirm receipt of $7 million as mentioned in previous finance agreement" xr:uid="{A2CAAC11-3AA2-4D99-B693-8505C47A6E02}"/>
+    <hyperlink ref="H25" r:id="rId3" display="2021 Malian coup d'etat begins led by the Malian Army &amp; Vice President of Mali" xr:uid="{98DA3C71-ACDA-5847-9BCE-1CF7AA6AF31A}"/>
+    <hyperlink ref="H11" r:id="rId4" xr:uid="{CFBE2DC5-BD46-4AEA-B124-0F71050A4DEA}"/>
+    <hyperlink ref="H9" r:id="rId5" display="Kodal Minerals confirm receipt of $7 million as mentioned in previous finance agreement" xr:uid="{A2CAAC11-3AA2-4D99-B693-8505C47A6E02}"/>
+    <hyperlink ref="H7" r:id="rId6" xr:uid="{4F95A3C1-2DBB-4F64-81EA-BE641A62ED90}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
-  <drawing r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+  <drawing r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>